<commit_message>
o tal das 6 da tarde
</commit_message>
<xml_diff>
--- a/Dataset_Wheater.xlsx
+++ b/Dataset_Wheater.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Hackaton\os-colegas-da-francisca\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8227F10A-0D3E-489A-9B5E-7B47B9BFFD6E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B454DE43-714D-42BC-BEAD-E5463D64A808}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Glass" sheetId="1" r:id="rId1"/>
@@ -116,12 +116,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -136,7 +148,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -178,6 +190,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -460,8 +476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F37" sqref="F37:F43"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -603,7 +619,7 @@
       <c r="D3" s="3">
         <v>52467.620000019298</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="41">
         <v>0.161008521870737</v>
       </c>
       <c r="F3" s="30">
@@ -659,7 +675,7 @@
       <c r="D4" s="3">
         <v>104194.060000001</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="41">
         <v>0.31974256862241701</v>
       </c>
       <c r="F4" s="30">
@@ -715,7 +731,7 @@
       <c r="D5" s="3">
         <v>72456.099999982995</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="41">
         <v>0.22234760336968301</v>
       </c>
       <c r="F5" s="30">
@@ -995,7 +1011,7 @@
       <c r="D10" s="5">
         <v>35730.560000017598</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="41">
         <v>0.18198702987114099</v>
       </c>
       <c r="F10" s="31">
@@ -1051,7 +1067,7 @@
       <c r="D11" s="5">
         <v>56778.519999981399</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="41">
         <v>0.28919093950026897</v>
       </c>
       <c r="F11" s="31">
@@ -1107,7 +1123,7 @@
       <c r="D12" s="5">
         <v>44826.989999991303</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="41">
         <v>0.228318021552356</v>
       </c>
       <c r="F12" s="31">
@@ -1387,7 +1403,7 @@
       <c r="D17" s="8">
         <v>21508.029999994102</v>
       </c>
-      <c r="E17" s="9">
+      <c r="E17" s="41">
         <v>0.177720368446146</v>
       </c>
       <c r="F17" s="32">
@@ -1443,7 +1459,7 @@
       <c r="D18" s="8">
         <v>45240.700000008197</v>
       </c>
-      <c r="E18" s="9">
+      <c r="E18" s="41">
         <v>0.373822887208415</v>
       </c>
       <c r="F18" s="32">
@@ -1499,7 +1515,7 @@
       <c r="D19" s="8">
         <v>20409.319999998199</v>
       </c>
-      <c r="E19" s="9">
+      <c r="E19" s="41">
         <v>0.16864175241228399</v>
       </c>
       <c r="F19" s="32">
@@ -1779,7 +1795,7 @@
       <c r="D24" s="10">
         <v>10171.6600000159</v>
       </c>
-      <c r="E24" s="11">
+      <c r="E24" s="41">
         <v>0.17558951420064101</v>
       </c>
       <c r="F24" s="33">
@@ -1835,7 +1851,7 @@
       <c r="D25" s="10">
         <v>20902.6699999882</v>
       </c>
-      <c r="E25" s="11">
+      <c r="E25" s="41">
         <v>0.360834875604229</v>
       </c>
       <c r="F25" s="33">
@@ -1891,7 +1907,7 @@
       <c r="D26" s="10">
         <v>11141.050000028599</v>
       </c>
-      <c r="E26" s="11">
+      <c r="E26" s="41">
         <v>0.19232372662741501</v>
       </c>
       <c r="F26" s="33">
@@ -2115,7 +2131,7 @@
       <c r="D30" s="12">
         <v>2586.1300000044198</v>
       </c>
-      <c r="E30" s="14">
+      <c r="E30" s="41">
         <v>0.19171898641667401</v>
       </c>
       <c r="F30" s="34">
@@ -2171,7 +2187,7 @@
       <c r="D31" s="12">
         <v>2700.9000000059</v>
       </c>
-      <c r="E31" s="14">
+      <c r="E31" s="41">
         <v>0.200227293451233</v>
       </c>
       <c r="F31" s="34">
@@ -2227,7 +2243,7 @@
       <c r="D32" s="12">
         <v>3716.8400000117299</v>
       </c>
-      <c r="E32" s="14">
+      <c r="E32" s="41">
         <v>0.275542527821099</v>
       </c>
       <c r="F32" s="34">
@@ -2283,7 +2299,7 @@
       <c r="D33" s="12">
         <v>2181.18999999567</v>
       </c>
-      <c r="E33" s="14">
+      <c r="E33" s="41">
         <v>0.16169934843980699</v>
       </c>
       <c r="F33" s="34">
@@ -2563,7 +2579,7 @@
       <c r="D38" s="15">
         <v>768.33999999096795</v>
       </c>
-      <c r="E38" s="17">
+      <c r="E38" s="41">
         <v>0.23082700442118201</v>
       </c>
       <c r="F38" s="34">
@@ -2619,7 +2635,7 @@
       <c r="D39" s="15">
         <v>1232.48999999635</v>
       </c>
-      <c r="E39" s="17">
+      <c r="E39" s="41">
         <v>0.37026833782123098</v>
       </c>
       <c r="F39" s="34">
@@ -2675,7 +2691,7 @@
       <c r="D40" s="15">
         <v>367.41999999097197</v>
       </c>
-      <c r="E40" s="17">
+      <c r="E40" s="41">
         <v>0.11038141703327101</v>
       </c>
       <c r="F40" s="34">
@@ -2895,8 +2911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4412D37-A799-4C1C-BDF0-1B2C7F8B9CD8}">
   <dimension ref="A1:Z43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2908,6 +2924,7 @@
     <col min="5" max="5" width="26" customWidth="1"/>
     <col min="6" max="6" width="27.140625" customWidth="1"/>
     <col min="7" max="7" width="17" customWidth="1"/>
+    <col min="13" max="13" width="13" customWidth="1"/>
     <col min="17" max="17" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3036,7 +3053,7 @@
       <c r="D3" s="18">
         <v>20669.819999977499</v>
       </c>
-      <c r="E3" s="19">
+      <c r="E3" s="41">
         <v>0.15792085349212301</v>
       </c>
       <c r="F3" s="35">
@@ -3092,7 +3109,7 @@
       <c r="D4" s="18">
         <v>40395.160000003198</v>
       </c>
-      <c r="E4" s="19">
+      <c r="E4" s="41">
         <v>0.29851548608526701</v>
       </c>
       <c r="F4" s="35">
@@ -3148,7 +3165,7 @@
       <c r="D5" s="18">
         <v>30237.390000013202</v>
       </c>
-      <c r="E5" s="19">
+      <c r="E5" s="41">
         <v>0.22375222263573599</v>
       </c>
       <c r="F5" s="35">
@@ -3444,7 +3461,7 @@
       <c r="D10" s="20">
         <v>15015.7699999957</v>
       </c>
-      <c r="E10" s="21">
+      <c r="E10" s="41">
         <v>0.189107827038862</v>
       </c>
       <c r="F10" s="36">
@@ -3508,7 +3525,7 @@
       <c r="D11" s="20">
         <v>22444.1100000201</v>
       </c>
-      <c r="E11" s="21">
+      <c r="E11" s="41">
         <v>0.27565681444991802</v>
       </c>
       <c r="F11" s="36">
@@ -3564,7 +3581,7 @@
       <c r="D12" s="20">
         <v>17341.090000003602</v>
       </c>
-      <c r="E12" s="21">
+      <c r="E12" s="41">
         <v>0.212848932676519</v>
       </c>
       <c r="F12" s="36">
@@ -3868,7 +3885,7 @@
       <c r="D17" s="22">
         <v>7966.38000000584</v>
       </c>
-      <c r="E17" s="23">
+      <c r="E17" s="41">
         <v>0.17922303586943</v>
       </c>
       <c r="F17" s="37">
@@ -3924,7 +3941,7 @@
       <c r="D18" s="22">
         <v>14037.380000024899</v>
       </c>
-      <c r="E18" s="23">
+      <c r="E18" s="41">
         <v>0.31289561871664401</v>
       </c>
       <c r="F18" s="37">
@@ -3988,7 +4005,7 @@
       <c r="D19" s="22">
         <v>7333.3800000208003</v>
       </c>
-      <c r="E19" s="23">
+      <c r="E19" s="41">
         <v>0.16209507260767</v>
       </c>
       <c r="F19" s="37">
@@ -4284,7 +4301,7 @@
       <c r="D24" s="24">
         <v>2579.72000000463</v>
       </c>
-      <c r="E24" s="25">
+      <c r="E24" s="41">
         <v>0.19003984063745</v>
       </c>
       <c r="F24" s="38">
@@ -4348,7 +4365,7 @@
       <c r="D25" s="24">
         <v>4517.1100000133702</v>
       </c>
-      <c r="E25" s="25">
+      <c r="E25" s="41">
         <v>0.31434262948207198</v>
       </c>
       <c r="F25" s="38">
@@ -4404,7 +4421,7 @@
       <c r="D26" s="24">
         <v>2498.5600000025001</v>
       </c>
-      <c r="E26" s="25">
+      <c r="E26" s="41">
         <v>0.17211155378486101</v>
       </c>
       <c r="F26" s="38">
@@ -4632,58 +4649,58 @@
       <c r="Z29" s="29"/>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
+      <c r="A30" s="42">
         <v>43510</v>
       </c>
-      <c r="B30" s="16" t="s">
+      <c r="B30" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="C30" s="16">
+      <c r="C30" s="43">
         <v>5</v>
       </c>
-      <c r="D30" s="26">
+      <c r="D30" s="43">
         <v>925.920000002954</v>
       </c>
-      <c r="E30" s="27">
+      <c r="E30" s="44">
         <v>0.116642958748222</v>
       </c>
-      <c r="F30" s="39">
+      <c r="F30" s="43">
         <v>7839.4899999872496</v>
       </c>
-      <c r="G30" s="16">
+      <c r="G30" s="43">
         <v>70</v>
       </c>
-      <c r="H30" s="16">
+      <c r="H30" s="43">
         <v>50</v>
       </c>
-      <c r="I30" s="16">
-        <v>0</v>
-      </c>
-      <c r="J30" s="16">
-        <v>58</v>
-      </c>
-      <c r="K30" s="16">
+      <c r="I30" s="43">
+        <v>0</v>
+      </c>
+      <c r="J30" s="43">
+        <v>58</v>
+      </c>
+      <c r="K30" s="43">
         <v>41</v>
       </c>
-      <c r="L30" s="16">
-        <v>0</v>
-      </c>
-      <c r="M30" s="16">
+      <c r="L30" s="43">
+        <v>0</v>
+      </c>
+      <c r="M30" s="43">
         <v>66</v>
       </c>
-      <c r="N30" s="16">
-        <v>46</v>
-      </c>
-      <c r="O30" s="16">
-        <v>0</v>
-      </c>
-      <c r="P30" s="16">
-        <v>58</v>
-      </c>
-      <c r="Q30" s="16">
-        <v>47</v>
-      </c>
-      <c r="R30" s="16">
+      <c r="N30" s="43">
+        <v>46</v>
+      </c>
+      <c r="O30" s="43">
+        <v>0</v>
+      </c>
+      <c r="P30" s="43">
+        <v>58</v>
+      </c>
+      <c r="Q30" s="43">
+        <v>47</v>
+      </c>
+      <c r="R30" s="43">
         <v>0</v>
       </c>
     </row>
@@ -4756,7 +4773,7 @@
       <c r="D32" s="26">
         <v>2388.7100000123201</v>
       </c>
-      <c r="E32" s="27">
+      <c r="E32" s="41">
         <v>0.29302987197724001</v>
       </c>
       <c r="F32" s="39">
@@ -4812,7 +4829,7 @@
       <c r="D33" s="26">
         <v>1468.7300000012201</v>
       </c>
-      <c r="E33" s="27">
+      <c r="E33" s="41">
         <v>0.17567567567567599</v>
       </c>
       <c r="F33" s="39">
@@ -4856,58 +4873,58 @@
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
+      <c r="A34" s="42">
         <v>43514</v>
       </c>
-      <c r="B34" s="16" t="s">
+      <c r="B34" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="C34" s="16">
+      <c r="C34" s="43">
         <v>5</v>
       </c>
-      <c r="D34" s="26">
+      <c r="D34" s="43">
         <v>960.89999999244696</v>
       </c>
-      <c r="E34" s="27">
+      <c r="E34" s="44">
         <v>0.139402560455192</v>
       </c>
-      <c r="F34" s="39">
+      <c r="F34" s="43">
         <v>7839.4899999872496</v>
       </c>
-      <c r="G34" s="16">
+      <c r="G34" s="43">
         <v>59</v>
       </c>
-      <c r="H34" s="16">
+      <c r="H34" s="43">
         <v>45</v>
       </c>
-      <c r="I34" s="16">
+      <c r="I34" s="43">
         <v>0.3</v>
       </c>
-      <c r="J34" s="16">
-        <v>58</v>
-      </c>
-      <c r="K34" s="16">
+      <c r="J34" s="43">
+        <v>58</v>
+      </c>
+      <c r="K34" s="43">
         <v>42</v>
       </c>
-      <c r="L34" s="16">
-        <v>0</v>
-      </c>
-      <c r="M34" s="16">
+      <c r="L34" s="43">
+        <v>0</v>
+      </c>
+      <c r="M34" s="43">
         <v>54</v>
       </c>
-      <c r="N34" s="16">
+      <c r="N34" s="43">
         <v>48</v>
       </c>
-      <c r="O34" s="16">
-        <v>0</v>
-      </c>
-      <c r="P34" s="16">
-        <v>58</v>
-      </c>
-      <c r="Q34" s="16">
-        <v>47</v>
-      </c>
-      <c r="R34" s="16">
+      <c r="O34" s="43">
+        <v>0</v>
+      </c>
+      <c r="P34" s="43">
+        <v>58</v>
+      </c>
+      <c r="Q34" s="43">
+        <v>47</v>
+      </c>
+      <c r="R34" s="43">
         <v>0</v>
       </c>
     </row>
@@ -5092,7 +5109,7 @@
       <c r="D38" s="28">
         <v>881.74000000072999</v>
       </c>
-      <c r="E38" s="29">
+      <c r="E38" s="41">
         <v>0.14367269267364399</v>
       </c>
       <c r="F38" s="40">
@@ -5148,7 +5165,7 @@
       <c r="D39" s="28">
         <v>1348.8000000028901</v>
       </c>
-      <c r="E39" s="29">
+      <c r="E39" s="41">
         <v>0.22359657469077099</v>
       </c>
       <c r="F39" s="40">
@@ -5204,7 +5221,7 @@
       <c r="D40" s="28">
         <v>1004.27999998993</v>
       </c>
-      <c r="E40" s="29">
+      <c r="E40" s="41">
         <v>0.16365366317792601</v>
       </c>
       <c r="F40" s="40">
@@ -5248,58 +5265,58 @@
       </c>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A41" s="1">
+      <c r="A41" s="42">
         <v>43521</v>
       </c>
-      <c r="B41" s="16" t="s">
+      <c r="B41" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="C41" s="16">
+      <c r="C41" s="43">
         <v>6</v>
       </c>
-      <c r="D41" s="28">
+      <c r="D41" s="43">
         <v>965.35000000174398</v>
       </c>
-      <c r="E41" s="29">
+      <c r="E41" s="44">
         <v>0.19219790675547099</v>
       </c>
-      <c r="F41" s="40">
+      <c r="F41" s="43">
         <v>5638.6199999970104</v>
       </c>
-      <c r="G41" s="16">
+      <c r="G41" s="43">
         <v>74</v>
       </c>
-      <c r="H41" s="16">
+      <c r="H41" s="43">
         <v>53</v>
       </c>
-      <c r="I41" s="16">
-        <v>0</v>
-      </c>
-      <c r="J41" s="16">
+      <c r="I41" s="43">
+        <v>0</v>
+      </c>
+      <c r="J41" s="43">
         <v>59</v>
       </c>
-      <c r="K41" s="16">
+      <c r="K41" s="43">
         <v>43</v>
       </c>
-      <c r="L41" s="16">
-        <v>0</v>
-      </c>
-      <c r="M41" s="16">
+      <c r="L41" s="43">
+        <v>0</v>
+      </c>
+      <c r="M41" s="43">
         <v>72</v>
       </c>
-      <c r="N41" s="16">
+      <c r="N41" s="43">
         <v>48</v>
       </c>
-      <c r="O41" s="16">
-        <v>0</v>
-      </c>
-      <c r="P41" s="16">
+      <c r="O41" s="43">
+        <v>0</v>
+      </c>
+      <c r="P41" s="43">
         <v>59</v>
       </c>
-      <c r="Q41" s="16">
-        <v>47</v>
-      </c>
-      <c r="R41" s="16">
+      <c r="Q41" s="43">
+        <v>47</v>
+      </c>
+      <c r="R41" s="43">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
models, processes and photos
</commit_message>
<xml_diff>
--- a/Dataset_Wheater.xlsx
+++ b/Dataset_Wheater.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Hackaton\os-colegas-da-francisca\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B454DE43-714D-42BC-BEAD-E5463D64A808}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F78781D1-4E50-4E43-A5FE-3F7AA794BDD6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Glass" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="25">
   <si>
     <t>Day</t>
   </si>
@@ -107,7 +107,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,8 +115,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -135,6 +143,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -148,7 +162,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -188,12 +202,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -476,8 +492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -619,7 +635,7 @@
       <c r="D3" s="3">
         <v>52467.620000019298</v>
       </c>
-      <c r="E3" s="41">
+      <c r="E3" s="39">
         <v>0.161008521870737</v>
       </c>
       <c r="F3" s="30">
@@ -675,7 +691,7 @@
       <c r="D4" s="3">
         <v>104194.060000001</v>
       </c>
-      <c r="E4" s="41">
+      <c r="E4" s="39">
         <v>0.31974256862241701</v>
       </c>
       <c r="F4" s="30">
@@ -731,7 +747,7 @@
       <c r="D5" s="3">
         <v>72456.099999982995</v>
       </c>
-      <c r="E5" s="41">
+      <c r="E5" s="39">
         <v>0.22234760336968301</v>
       </c>
       <c r="F5" s="30">
@@ -1011,7 +1027,7 @@
       <c r="D10" s="5">
         <v>35730.560000017598</v>
       </c>
-      <c r="E10" s="41">
+      <c r="E10" s="39">
         <v>0.18198702987114099</v>
       </c>
       <c r="F10" s="31">
@@ -1067,7 +1083,7 @@
       <c r="D11" s="5">
         <v>56778.519999981399</v>
       </c>
-      <c r="E11" s="41">
+      <c r="E11" s="39">
         <v>0.28919093950026897</v>
       </c>
       <c r="F11" s="31">
@@ -1123,7 +1139,7 @@
       <c r="D12" s="5">
         <v>44826.989999991303</v>
       </c>
-      <c r="E12" s="41">
+      <c r="E12" s="39">
         <v>0.228318021552356</v>
       </c>
       <c r="F12" s="31">
@@ -1403,7 +1419,7 @@
       <c r="D17" s="8">
         <v>21508.029999994102</v>
       </c>
-      <c r="E17" s="41">
+      <c r="E17" s="39">
         <v>0.177720368446146</v>
       </c>
       <c r="F17" s="32">
@@ -1459,7 +1475,7 @@
       <c r="D18" s="8">
         <v>45240.700000008197</v>
       </c>
-      <c r="E18" s="41">
+      <c r="E18" s="39">
         <v>0.373822887208415</v>
       </c>
       <c r="F18" s="32">
@@ -1515,7 +1531,7 @@
       <c r="D19" s="8">
         <v>20409.319999998199</v>
       </c>
-      <c r="E19" s="41">
+      <c r="E19" s="39">
         <v>0.16864175241228399</v>
       </c>
       <c r="F19" s="32">
@@ -1795,7 +1811,7 @@
       <c r="D24" s="10">
         <v>10171.6600000159</v>
       </c>
-      <c r="E24" s="41">
+      <c r="E24" s="39">
         <v>0.17558951420064101</v>
       </c>
       <c r="F24" s="33">
@@ -1851,7 +1867,7 @@
       <c r="D25" s="10">
         <v>20902.6699999882</v>
       </c>
-      <c r="E25" s="41">
+      <c r="E25" s="39">
         <v>0.360834875604229</v>
       </c>
       <c r="F25" s="33">
@@ -1907,7 +1923,7 @@
       <c r="D26" s="10">
         <v>11141.050000028599</v>
       </c>
-      <c r="E26" s="41">
+      <c r="E26" s="39">
         <v>0.19232372662741501</v>
       </c>
       <c r="F26" s="33">
@@ -2119,58 +2135,58 @@
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
+      <c r="A30" s="43">
         <v>43510</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="44">
         <v>5</v>
       </c>
-      <c r="D30" s="12">
+      <c r="D30" s="44">
         <v>2586.1300000044198</v>
       </c>
-      <c r="E30" s="41">
+      <c r="E30" s="45">
         <v>0.19171898641667401</v>
       </c>
-      <c r="F30" s="34">
+      <c r="F30" s="44">
         <v>13489.170000002699</v>
       </c>
-      <c r="G30" s="16">
+      <c r="G30" s="44">
         <v>70</v>
       </c>
-      <c r="H30" s="16">
+      <c r="H30" s="44">
         <v>50</v>
       </c>
-      <c r="I30" s="16">
-        <v>0</v>
-      </c>
-      <c r="J30" s="16">
-        <v>58</v>
-      </c>
-      <c r="K30" s="16">
+      <c r="I30" s="44">
+        <v>0</v>
+      </c>
+      <c r="J30" s="44">
+        <v>58</v>
+      </c>
+      <c r="K30" s="44">
         <v>41</v>
       </c>
-      <c r="L30" s="16">
-        <v>0</v>
-      </c>
-      <c r="M30" s="16">
+      <c r="L30" s="44">
+        <v>0</v>
+      </c>
+      <c r="M30" s="44">
         <v>66</v>
       </c>
-      <c r="N30" s="16">
+      <c r="N30" s="44">
         <v>46</v>
       </c>
-      <c r="O30" s="16">
-        <v>0</v>
-      </c>
-      <c r="P30" s="16">
-        <v>58</v>
-      </c>
-      <c r="Q30" s="16">
-        <v>47</v>
-      </c>
-      <c r="R30" s="16">
+      <c r="O30" s="44">
+        <v>0</v>
+      </c>
+      <c r="P30" s="44">
+        <v>58</v>
+      </c>
+      <c r="Q30" s="44">
+        <v>47</v>
+      </c>
+      <c r="R30" s="44">
         <v>0</v>
       </c>
     </row>
@@ -2187,7 +2203,7 @@
       <c r="D31" s="12">
         <v>2700.9000000059</v>
       </c>
-      <c r="E31" s="41">
+      <c r="E31" s="39">
         <v>0.200227293451233</v>
       </c>
       <c r="F31" s="34">
@@ -2243,7 +2259,7 @@
       <c r="D32" s="12">
         <v>3716.8400000117299</v>
       </c>
-      <c r="E32" s="41">
+      <c r="E32" s="39">
         <v>0.275542527821099</v>
       </c>
       <c r="F32" s="34">
@@ -2299,7 +2315,7 @@
       <c r="D33" s="12">
         <v>2181.18999999567</v>
       </c>
-      <c r="E33" s="41">
+      <c r="E33" s="39">
         <v>0.16169934843980699</v>
       </c>
       <c r="F33" s="34">
@@ -2579,7 +2595,7 @@
       <c r="D38" s="15">
         <v>768.33999999096795</v>
       </c>
-      <c r="E38" s="41">
+      <c r="E38" s="39">
         <v>0.23082700442118201</v>
       </c>
       <c r="F38" s="34">
@@ -2635,7 +2651,7 @@
       <c r="D39" s="15">
         <v>1232.48999999635</v>
       </c>
-      <c r="E39" s="41">
+      <c r="E39" s="39">
         <v>0.37026833782123098</v>
       </c>
       <c r="F39" s="34">
@@ -2691,7 +2707,7 @@
       <c r="D40" s="15">
         <v>367.41999999097197</v>
       </c>
-      <c r="E40" s="41">
+      <c r="E40" s="39">
         <v>0.11038141703327101</v>
       </c>
       <c r="F40" s="34">
@@ -2909,211 +2925,220 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4412D37-A799-4C1C-BDF0-1B2C7F8B9CD8}">
-  <dimension ref="A1:Z43"/>
+  <dimension ref="A1:Z29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27:G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" customWidth="1"/>
-    <col min="4" max="4" width="20.85546875" customWidth="1"/>
-    <col min="5" max="5" width="26" customWidth="1"/>
-    <col min="6" max="6" width="27.140625" customWidth="1"/>
-    <col min="7" max="7" width="17" customWidth="1"/>
-    <col min="13" max="13" width="13" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="21.5703125" customWidth="1"/>
+    <col min="18" max="18" width="25.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="16" t="s">
+    <row r="1" spans="1:26" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="J1" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="16" t="s">
+      <c r="K1" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="L1" s="16" t="s">
+      <c r="L1" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="M1" s="16" t="s">
+      <c r="M1" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="N1" s="16" t="s">
+      <c r="N1" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="O1" s="16" t="s">
+      <c r="O1" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="P1" s="16" t="s">
+      <c r="P1" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" s="16" t="s">
+      <c r="Q1" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="R1" s="16" t="s">
+      <c r="R1" s="46" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>43482</v>
+        <v>43502</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C2" s="16">
-        <v>1</v>
-      </c>
-      <c r="D2" s="18">
-        <v>10024.719999996199</v>
-      </c>
-      <c r="E2" s="19">
-        <v>7.7657858826448295E-2</v>
+        <v>3</v>
+      </c>
+      <c r="D2" s="22">
+        <v>3301.1300000168299</v>
+      </c>
+      <c r="E2" s="23">
+        <v>7.5958793595631097E-2</v>
       </c>
       <c r="F2" s="35">
-        <v>132540.98999999199</v>
+        <v>44367.659999984397</v>
       </c>
       <c r="G2" s="16">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H2" s="16">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I2" s="16">
         <v>0</v>
       </c>
       <c r="J2" s="16">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="K2" s="16">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="L2" s="16">
         <v>0</v>
       </c>
       <c r="M2" s="16">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="N2" s="16">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="O2" s="16">
         <v>0</v>
       </c>
       <c r="P2" s="16">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="Q2" s="16">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="R2" s="16">
         <v>0</v>
       </c>
+      <c r="S2" s="26"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>43483</v>
+        <v>43503</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="16">
-        <v>1</v>
-      </c>
-      <c r="D3" s="18">
-        <v>20669.819999977499</v>
-      </c>
-      <c r="E3" s="41">
-        <v>0.15792085349212301</v>
-      </c>
-      <c r="F3" s="35">
-        <v>132540.98999999199</v>
+        <v>4</v>
+      </c>
+      <c r="D3" s="24">
+        <v>1155.59999999918</v>
+      </c>
+      <c r="E3" s="25">
+        <v>9.00398406374502E-2</v>
+      </c>
+      <c r="F3" s="36">
+        <v>13881.470000005</v>
       </c>
       <c r="G3" s="16">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="H3" s="16">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="I3" s="16">
-        <v>0.21</v>
+        <v>0</v>
       </c>
       <c r="J3" s="16">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="K3" s="16">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="L3" s="16">
         <v>0</v>
       </c>
       <c r="M3" s="16">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="N3" s="16">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O3" s="16">
         <v>0</v>
       </c>
       <c r="P3" s="16">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="Q3" s="16">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="R3" s="16">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>43484</v>
+        <v>43504</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="16">
-        <v>1</v>
-      </c>
-      <c r="D4" s="18">
-        <v>40395.160000003198</v>
-      </c>
-      <c r="E4" s="41">
-        <v>0.29851548608526701</v>
-      </c>
-      <c r="F4" s="35">
-        <v>132540.98999999199</v>
+        <v>4</v>
+      </c>
+      <c r="D4" s="24">
+        <v>2579.72000000463</v>
+      </c>
+      <c r="E4" s="39">
+        <v>0.19003984063745</v>
+      </c>
+      <c r="F4" s="36">
+        <v>13881.470000005</v>
       </c>
       <c r="G4" s="16">
         <v>58</v>
@@ -3122,92 +3147,92 @@
         <v>44</v>
       </c>
       <c r="I4" s="16">
-        <v>1.28</v>
+        <v>0.09</v>
       </c>
       <c r="J4" s="16">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="K4" s="16">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="L4" s="16">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="M4" s="16">
         <v>59</v>
       </c>
       <c r="N4" s="16">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="O4" s="16">
         <v>0</v>
       </c>
       <c r="P4" s="16">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="Q4" s="16">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="R4" s="16">
         <v>0</v>
       </c>
+      <c r="S4" s="27"/>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>43485</v>
+        <v>43505</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="16">
-        <v>1</v>
-      </c>
-      <c r="D5" s="18">
-        <v>30237.390000013202</v>
-      </c>
-      <c r="E5" s="41">
-        <v>0.22375222263573599</v>
-      </c>
-      <c r="F5" s="35">
-        <v>132540.98999999199</v>
+        <v>4</v>
+      </c>
+      <c r="D5" s="24">
+        <v>4517.1100000133702</v>
+      </c>
+      <c r="E5" s="39">
+        <v>0.31434262948207198</v>
+      </c>
+      <c r="F5" s="36">
+        <v>13881.470000005</v>
       </c>
       <c r="G5" s="16">
         <v>58</v>
       </c>
       <c r="H5" s="16">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="I5" s="16">
-        <v>0.02</v>
+        <v>0.16</v>
       </c>
       <c r="J5" s="16">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="K5" s="16">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="L5" s="16">
         <v>0</v>
       </c>
       <c r="M5" s="16">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="N5" s="16">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="O5" s="16">
         <v>0</v>
       </c>
       <c r="P5" s="16">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="Q5" s="16">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="R5" s="16">
-        <v>0.01</v>
-      </c>
-      <c r="S5" s="18"/>
+        <v>0</v>
+      </c>
       <c r="T5" s="18"/>
       <c r="U5" s="18"/>
       <c r="V5" s="18"/>
@@ -3218,99 +3243,100 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>43486</v>
+        <v>43506</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" s="16">
-        <v>1</v>
-      </c>
-      <c r="D6" s="18">
-        <v>11403.510000018099</v>
-      </c>
-      <c r="E6" s="19">
-        <v>8.8988132158954597E-2</v>
-      </c>
-      <c r="F6" s="35">
-        <v>132540.98999999199</v>
+        <v>4</v>
+      </c>
+      <c r="D6" s="24">
+        <v>2498.5600000025001</v>
+      </c>
+      <c r="E6" s="39">
+        <v>0.17211155378486101</v>
+      </c>
+      <c r="F6" s="36">
+        <v>13881.470000005</v>
       </c>
       <c r="G6" s="16">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H6" s="16">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="I6" s="16">
-        <v>0</v>
+        <v>1.32</v>
       </c>
       <c r="J6" s="16">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="K6" s="16">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="L6" s="16">
         <v>0</v>
       </c>
       <c r="M6" s="16">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="N6" s="16">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="O6" s="16">
         <v>0</v>
       </c>
       <c r="P6" s="16">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="Q6" s="16">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="R6" s="16">
         <v>0</v>
       </c>
+      <c r="S6" s="28"/>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>43487</v>
+        <v>43507</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="16">
-        <v>1</v>
-      </c>
-      <c r="D7" s="18">
-        <v>9250.0599999965107</v>
-      </c>
-      <c r="E7" s="19">
-        <v>6.9718397221188402E-2</v>
-      </c>
-      <c r="F7" s="35">
-        <v>132540.98999999199</v>
+        <v>4</v>
+      </c>
+      <c r="D7" s="24">
+        <v>1142.9499999990801</v>
+      </c>
+      <c r="E7" s="25">
+        <v>8.4063745019920297E-2</v>
+      </c>
+      <c r="F7" s="36">
+        <v>13881.470000005</v>
       </c>
       <c r="G7" s="16">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="H7" s="16">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="I7" s="16">
-        <v>0.26</v>
+        <v>0</v>
       </c>
       <c r="J7" s="16">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="K7" s="16">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="L7" s="16">
         <v>0</v>
       </c>
       <c r="M7" s="16">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="N7" s="16">
         <v>46</v>
@@ -3319,71 +3345,70 @@
         <v>0</v>
       </c>
       <c r="P7" s="16">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="Q7" s="16">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="R7" s="16">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>43488</v>
+        <v>43508</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" s="16">
-        <v>1</v>
-      </c>
-      <c r="D8" s="18">
-        <v>10560.330000022401</v>
-      </c>
-      <c r="E8" s="19">
-        <v>8.3447049580283705E-2</v>
-      </c>
-      <c r="F8" s="35">
-        <v>132540.98999999199</v>
+        <v>4</v>
+      </c>
+      <c r="D8" s="24">
+        <v>1002.49999999639</v>
+      </c>
+      <c r="E8" s="25">
+        <v>7.2908366533864497E-2</v>
+      </c>
+      <c r="F8" s="36">
+        <v>13881.470000005</v>
       </c>
       <c r="G8" s="16">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="H8" s="16">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="I8" s="16">
-        <v>0.24</v>
+        <v>0</v>
       </c>
       <c r="J8" s="16">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="K8" s="16">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="L8" s="16">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="M8" s="16">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="N8" s="16">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="O8" s="16">
         <v>0</v>
       </c>
       <c r="P8" s="16">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="Q8" s="16">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="R8" s="16">
         <v>0</v>
       </c>
-      <c r="S8" s="19"/>
       <c r="T8" s="19"/>
       <c r="U8" s="19"/>
       <c r="V8" s="19"/>
@@ -3394,116 +3419,116 @@
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>43489</v>
+        <v>43509</v>
       </c>
       <c r="B9" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="16">
         <v>4</v>
       </c>
-      <c r="C9" s="16">
-        <v>2</v>
-      </c>
-      <c r="D9" s="20">
-        <v>7953.68999998653</v>
-      </c>
-      <c r="E9" s="21">
-        <v>0.100095785440613</v>
+      <c r="D9" s="24">
+        <v>985.02999998989696</v>
+      </c>
+      <c r="E9" s="25">
+        <v>7.6494023904382494E-2</v>
       </c>
       <c r="F9" s="36">
-        <v>80113.020000020406</v>
+        <v>13881.470000005</v>
       </c>
       <c r="G9" s="16">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="H9" s="16">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="I9" s="16">
-        <v>0.09</v>
+        <v>0</v>
       </c>
       <c r="J9" s="16">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="K9" s="16">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="L9" s="16">
         <v>0</v>
       </c>
       <c r="M9" s="16">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="N9" s="16">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="O9" s="16">
         <v>0</v>
       </c>
       <c r="P9" s="16">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="Q9" s="16">
+        <v>47</v>
+      </c>
+      <c r="R9" s="16">
+        <v>0</v>
+      </c>
+      <c r="S9" s="29"/>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A10" s="40">
+        <v>43510</v>
+      </c>
+      <c r="B10" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="41">
+        <v>5</v>
+      </c>
+      <c r="D10" s="41">
+        <v>925.920000002954</v>
+      </c>
+      <c r="E10" s="42">
+        <v>0.116642958748222</v>
+      </c>
+      <c r="F10" s="41">
+        <v>7839.4899999872496</v>
+      </c>
+      <c r="G10" s="41">
+        <v>70</v>
+      </c>
+      <c r="H10" s="41">
+        <v>50</v>
+      </c>
+      <c r="I10" s="41">
+        <v>0</v>
+      </c>
+      <c r="J10" s="41">
+        <v>58</v>
+      </c>
+      <c r="K10" s="41">
+        <v>41</v>
+      </c>
+      <c r="L10" s="41">
+        <v>0</v>
+      </c>
+      <c r="M10" s="41">
+        <v>66</v>
+      </c>
+      <c r="N10" s="41">
         <v>46</v>
       </c>
-      <c r="R9" s="16">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>43490</v>
-      </c>
-      <c r="B10" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="16">
-        <v>2</v>
-      </c>
-      <c r="D10" s="20">
-        <v>15015.7699999957</v>
-      </c>
-      <c r="E10" s="41">
-        <v>0.189107827038862</v>
-      </c>
-      <c r="F10" s="36">
-        <v>80113.020000020406</v>
-      </c>
-      <c r="G10" s="16">
-        <v>64</v>
-      </c>
-      <c r="H10" s="16">
-        <v>42</v>
-      </c>
-      <c r="I10" s="16">
-        <v>0</v>
-      </c>
-      <c r="J10" s="16">
-        <v>57</v>
-      </c>
-      <c r="K10" s="16">
-        <v>40</v>
-      </c>
-      <c r="L10" s="16">
-        <v>0</v>
-      </c>
-      <c r="M10" s="16">
-        <v>66</v>
-      </c>
-      <c r="N10" s="16">
-        <v>50</v>
-      </c>
-      <c r="O10" s="16">
-        <v>0</v>
-      </c>
-      <c r="P10" s="16">
-        <v>56</v>
-      </c>
-      <c r="Q10" s="16">
-        <v>46</v>
-      </c>
-      <c r="R10" s="16">
-        <v>0</v>
-      </c>
-      <c r="S10" s="20"/>
+      <c r="O10" s="41">
+        <v>0</v>
+      </c>
+      <c r="P10" s="41">
+        <v>58</v>
+      </c>
+      <c r="Q10" s="41">
+        <v>47</v>
+      </c>
+      <c r="R10" s="41">
+        <v>0</v>
+      </c>
       <c r="T10" s="20"/>
       <c r="U10" s="20"/>
       <c r="V10" s="20"/>
@@ -3514,55 +3539,55 @@
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>43491</v>
+        <v>43511</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C11" s="16">
-        <v>2</v>
-      </c>
-      <c r="D11" s="20">
-        <v>22444.1100000201</v>
-      </c>
-      <c r="E11" s="41">
-        <v>0.27565681444991802</v>
-      </c>
-      <c r="F11" s="36">
-        <v>80113.020000020406</v>
+        <v>5</v>
+      </c>
+      <c r="D11" s="26">
+        <v>1003.94999999598</v>
+      </c>
+      <c r="E11" s="27">
+        <v>0.126600284495021</v>
+      </c>
+      <c r="F11" s="37">
+        <v>7839.4899999872496</v>
       </c>
       <c r="G11" s="16">
+        <v>66</v>
+      </c>
+      <c r="H11" s="16">
+        <v>49</v>
+      </c>
+      <c r="I11" s="16">
+        <v>0</v>
+      </c>
+      <c r="J11" s="16">
+        <v>58</v>
+      </c>
+      <c r="K11" s="16">
+        <v>41</v>
+      </c>
+      <c r="L11" s="16">
+        <v>0</v>
+      </c>
+      <c r="M11" s="16">
         <v>63</v>
       </c>
-      <c r="H11" s="16">
-        <v>47</v>
-      </c>
-      <c r="I11" s="16">
-        <v>0</v>
-      </c>
-      <c r="J11" s="16">
-        <v>57</v>
-      </c>
-      <c r="K11" s="16">
-        <v>40</v>
-      </c>
-      <c r="L11" s="16">
-        <v>0</v>
-      </c>
-      <c r="M11" s="16">
-        <v>64</v>
-      </c>
       <c r="N11" s="16">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="O11" s="16">
         <v>0</v>
       </c>
       <c r="P11" s="16">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="Q11" s="16">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="R11" s="16">
         <v>0.01</v>
@@ -3570,43 +3595,43 @@
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>43492</v>
+        <v>43512</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C12" s="16">
-        <v>2</v>
-      </c>
-      <c r="D12" s="20">
-        <v>17341.090000003602</v>
-      </c>
-      <c r="E12" s="41">
-        <v>0.212848932676519</v>
-      </c>
-      <c r="F12" s="36">
-        <v>80113.020000020406</v>
+        <v>5</v>
+      </c>
+      <c r="D12" s="26">
+        <v>2388.7100000123201</v>
+      </c>
+      <c r="E12" s="39">
+        <v>0.29302987197724001</v>
+      </c>
+      <c r="F12" s="37">
+        <v>7839.4899999872496</v>
       </c>
       <c r="G12" s="16">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="H12" s="16">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I12" s="16">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="J12" s="16">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="K12" s="16">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="L12" s="16">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="M12" s="16">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="N12" s="16">
         <v>50</v>
@@ -3615,15 +3640,14 @@
         <v>0</v>
       </c>
       <c r="P12" s="16">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="Q12" s="16">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="R12" s="16">
         <v>0</v>
       </c>
-      <c r="S12" s="21"/>
       <c r="T12" s="21"/>
       <c r="U12" s="21"/>
       <c r="V12" s="21"/>
@@ -3634,116 +3658,115 @@
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>43493</v>
+        <v>43513</v>
       </c>
       <c r="B13" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="16">
+        <v>5</v>
+      </c>
+      <c r="D13" s="26">
+        <v>1468.7300000012201</v>
+      </c>
+      <c r="E13" s="39">
+        <v>0.17567567567567599</v>
+      </c>
+      <c r="F13" s="37">
+        <v>7839.4899999872496</v>
+      </c>
+      <c r="G13" s="16">
+        <v>62</v>
+      </c>
+      <c r="H13" s="16">
+        <v>47</v>
+      </c>
+      <c r="I13" s="16">
+        <v>0.13</v>
+      </c>
+      <c r="J13" s="16">
+        <v>58</v>
+      </c>
+      <c r="K13" s="16">
+        <v>41</v>
+      </c>
+      <c r="L13" s="16">
+        <v>0</v>
+      </c>
+      <c r="M13" s="16">
+        <v>61</v>
+      </c>
+      <c r="N13" s="16">
+        <v>46</v>
+      </c>
+      <c r="O13" s="16">
+        <v>0</v>
+      </c>
+      <c r="P13" s="16">
+        <v>58</v>
+      </c>
+      <c r="Q13" s="16">
+        <v>47</v>
+      </c>
+      <c r="R13" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A14" s="40">
+        <v>43514</v>
+      </c>
+      <c r="B14" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="16">
-        <v>2</v>
-      </c>
-      <c r="D13" s="20">
-        <v>6533.9199999901502</v>
-      </c>
-      <c r="E13" s="21">
-        <v>8.3401751505199795E-2</v>
-      </c>
-      <c r="F13" s="36">
-        <v>80113.020000020406</v>
-      </c>
-      <c r="G13" s="16">
-        <v>58</v>
-      </c>
-      <c r="H13" s="16">
-        <v>46</v>
-      </c>
-      <c r="I13" s="16">
-        <v>0.12</v>
-      </c>
-      <c r="J13" s="16">
-        <v>57</v>
-      </c>
-      <c r="K13" s="16">
-        <v>40</v>
-      </c>
-      <c r="L13" s="16">
-        <v>0</v>
-      </c>
-      <c r="M13" s="16">
-        <v>57</v>
-      </c>
-      <c r="N13" s="16">
-        <v>50</v>
-      </c>
-      <c r="O13" s="16">
-        <v>0</v>
-      </c>
-      <c r="P13" s="16">
-        <v>56</v>
-      </c>
-      <c r="Q13" s="16">
-        <v>46</v>
-      </c>
-      <c r="R13" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>43494</v>
-      </c>
-      <c r="B14" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="16">
-        <v>2</v>
-      </c>
-      <c r="D14" s="20">
-        <v>5494.3999999932603</v>
-      </c>
-      <c r="E14" s="21">
-        <v>6.9718117131910201E-2</v>
-      </c>
-      <c r="F14" s="36">
-        <v>80113.020000020406</v>
-      </c>
-      <c r="G14" s="16">
-        <v>55</v>
-      </c>
-      <c r="H14" s="16">
-        <v>47</v>
-      </c>
-      <c r="I14" s="16">
-        <v>0.31</v>
-      </c>
-      <c r="J14" s="16">
-        <v>57</v>
-      </c>
-      <c r="K14" s="16">
-        <v>40</v>
-      </c>
-      <c r="L14" s="16">
-        <v>0</v>
-      </c>
-      <c r="M14" s="16">
-        <v>55</v>
-      </c>
-      <c r="N14" s="16">
-        <v>52</v>
-      </c>
-      <c r="O14" s="16">
-        <v>0</v>
-      </c>
-      <c r="P14" s="16">
-        <v>57</v>
-      </c>
-      <c r="Q14" s="16">
-        <v>46</v>
-      </c>
-      <c r="R14" s="16">
-        <v>0</v>
-      </c>
-      <c r="S14" s="22"/>
+      <c r="C14" s="41">
+        <v>5</v>
+      </c>
+      <c r="D14" s="41">
+        <v>960.89999999244696</v>
+      </c>
+      <c r="E14" s="42">
+        <v>0.139402560455192</v>
+      </c>
+      <c r="F14" s="41">
+        <v>7839.4899999872496</v>
+      </c>
+      <c r="G14" s="41">
+        <v>59</v>
+      </c>
+      <c r="H14" s="41">
+        <v>45</v>
+      </c>
+      <c r="I14" s="41">
+        <v>0.3</v>
+      </c>
+      <c r="J14" s="41">
+        <v>58</v>
+      </c>
+      <c r="K14" s="41">
+        <v>42</v>
+      </c>
+      <c r="L14" s="41">
+        <v>0</v>
+      </c>
+      <c r="M14" s="41">
+        <v>54</v>
+      </c>
+      <c r="N14" s="41">
+        <v>48</v>
+      </c>
+      <c r="O14" s="41">
+        <v>0</v>
+      </c>
+      <c r="P14" s="41">
+        <v>58</v>
+      </c>
+      <c r="Q14" s="41">
+        <v>47</v>
+      </c>
+      <c r="R14" s="41">
+        <v>0</v>
+      </c>
       <c r="T14" s="22"/>
       <c r="U14" s="22"/>
       <c r="V14" s="22"/>
@@ -3754,116 +3777,115 @@
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>43495</v>
+        <v>43515</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C15" s="16">
-        <v>2</v>
-      </c>
-      <c r="D15" s="20">
-        <v>5330.0399999783504</v>
-      </c>
-      <c r="E15" s="21">
-        <v>6.9170771756978694E-2</v>
-      </c>
-      <c r="F15" s="36">
-        <v>80113.020000020406</v>
+        <v>5</v>
+      </c>
+      <c r="D15" s="26">
+        <v>458.800000008724</v>
+      </c>
+      <c r="E15" s="27">
+        <v>6.1166429587482203E-2</v>
+      </c>
+      <c r="F15" s="37">
+        <v>7839.4899999872496</v>
       </c>
       <c r="G15" s="16">
         <v>56</v>
       </c>
       <c r="H15" s="16">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="I15" s="16">
-        <v>1.71</v>
+        <v>0</v>
       </c>
       <c r="J15" s="16">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="K15" s="16">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="L15" s="16">
         <v>0</v>
       </c>
       <c r="M15" s="16">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="N15" s="16">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="O15" s="16">
         <v>0</v>
       </c>
       <c r="P15" s="16">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="Q15" s="16">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="R15" s="16">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>43496</v>
+        <v>43516</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C16" s="16">
-        <v>3</v>
-      </c>
-      <c r="D16" s="22">
-        <v>4415.4300000187404</v>
-      </c>
-      <c r="E16" s="23">
-        <v>0.100906044433412</v>
+        <v>5</v>
+      </c>
+      <c r="D16" s="26">
+        <v>632.48000000912396</v>
+      </c>
+      <c r="E16" s="27">
+        <v>8.7482219061166405E-2</v>
       </c>
       <c r="F16" s="37">
-        <v>44367.659999984397</v>
+        <v>7839.4899999872496</v>
       </c>
       <c r="G16" s="16">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H16" s="16">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="I16" s="16">
-        <v>1.35</v>
+        <v>0</v>
       </c>
       <c r="J16" s="16">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="K16" s="16">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L16" s="16">
         <v>0.01</v>
       </c>
       <c r="M16" s="16">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="N16" s="16">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="O16" s="16">
         <v>0</v>
       </c>
       <c r="P16" s="16">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="Q16" s="16">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="R16" s="16">
         <v>0</v>
       </c>
-      <c r="S16" s="23"/>
       <c r="T16" s="23"/>
       <c r="U16" s="23"/>
       <c r="V16" s="23"/>
@@ -3874,116 +3896,115 @@
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>43497</v>
+        <v>43517</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C17" s="16">
-        <v>3</v>
-      </c>
-      <c r="D17" s="22">
-        <v>7966.38000000584</v>
-      </c>
-      <c r="E17" s="41">
-        <v>0.17922303586943</v>
-      </c>
-      <c r="F17" s="37">
-        <v>44367.659999984397</v>
+        <v>6</v>
+      </c>
+      <c r="D17" s="28">
+        <v>445.849999992432</v>
+      </c>
+      <c r="E17" s="29">
+        <v>7.9923882017126593E-2</v>
+      </c>
+      <c r="F17" s="38">
+        <v>5638.6199999970104</v>
       </c>
       <c r="G17" s="16">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="H17" s="16">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="I17" s="16">
-        <v>0.74</v>
+        <v>0</v>
       </c>
       <c r="J17" s="16">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="K17" s="16">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L17" s="16">
-        <v>0.21</v>
+        <v>0</v>
       </c>
       <c r="M17" s="16">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="N17" s="16">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="O17" s="16">
         <v>0</v>
       </c>
       <c r="P17" s="16">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="Q17" s="16">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="R17" s="16">
-        <v>0.12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>43498</v>
+        <v>43518</v>
       </c>
       <c r="B18" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="16">
         <v>6</v>
       </c>
-      <c r="C18" s="16">
-        <v>3</v>
-      </c>
-      <c r="D18" s="22">
-        <v>14037.380000024899</v>
-      </c>
-      <c r="E18" s="41">
-        <v>0.31289561871664401</v>
-      </c>
-      <c r="F18" s="37">
-        <v>44367.659999984397</v>
+      <c r="D18" s="28">
+        <v>881.74000000072999</v>
+      </c>
+      <c r="E18" s="39">
+        <v>0.14367269267364399</v>
+      </c>
+      <c r="F18" s="38">
+        <v>5638.6199999970104</v>
       </c>
       <c r="G18" s="16">
-        <v>54</v>
+        <v>73</v>
       </c>
       <c r="H18" s="16">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="I18" s="16">
-        <v>0.18</v>
+        <v>0</v>
       </c>
       <c r="J18" s="16">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="K18" s="16">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L18" s="16">
         <v>0</v>
       </c>
       <c r="M18" s="16">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="N18" s="16">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="O18" s="16">
         <v>0</v>
       </c>
       <c r="P18" s="16">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="Q18" s="16">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="R18" s="16">
-        <v>0</v>
-      </c>
-      <c r="S18" s="24"/>
+        <v>0.01</v>
+      </c>
       <c r="T18" s="24"/>
       <c r="U18" s="24"/>
       <c r="V18" s="24"/>
@@ -3994,55 +4015,55 @@
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>43499</v>
+        <v>43519</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C19" s="16">
-        <v>3</v>
-      </c>
-      <c r="D19" s="22">
-        <v>7333.3800000208003</v>
-      </c>
-      <c r="E19" s="41">
-        <v>0.16209507260767</v>
-      </c>
-      <c r="F19" s="37">
-        <v>44367.659999984397</v>
+        <v>6</v>
+      </c>
+      <c r="D19" s="28">
+        <v>1348.8000000028901</v>
+      </c>
+      <c r="E19" s="39">
+        <v>0.22359657469077099</v>
+      </c>
+      <c r="F19" s="38">
+        <v>5638.6199999970104</v>
       </c>
       <c r="G19" s="16">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="H19" s="16">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="I19" s="16">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="J19" s="16">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="K19" s="16">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L19" s="16">
         <v>0</v>
       </c>
       <c r="M19" s="16">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="N19" s="16">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="O19" s="16">
         <v>0</v>
       </c>
       <c r="P19" s="16">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="Q19" s="16">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="R19" s="16">
         <v>0</v>
@@ -4050,60 +4071,59 @@
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>43500</v>
+        <v>43520</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C20" s="16">
-        <v>3</v>
-      </c>
-      <c r="D20" s="22">
-        <v>3825.10999999264</v>
-      </c>
-      <c r="E20" s="23">
-        <v>8.8990939555665893E-2</v>
-      </c>
-      <c r="F20" s="37">
-        <v>44367.659999984397</v>
+        <v>6</v>
+      </c>
+      <c r="D20" s="28">
+        <v>1004.27999998993</v>
+      </c>
+      <c r="E20" s="39">
+        <v>0.16365366317792601</v>
+      </c>
+      <c r="F20" s="38">
+        <v>5638.6199999970104</v>
       </c>
       <c r="G20" s="16">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="H20" s="16">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="I20" s="16">
         <v>0</v>
       </c>
       <c r="J20" s="16">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="K20" s="16">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="L20" s="16">
         <v>0.01</v>
       </c>
       <c r="M20" s="16">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="N20" s="16">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="O20" s="16">
         <v>0</v>
       </c>
       <c r="P20" s="16">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="Q20" s="16">
         <v>47</v>
       </c>
       <c r="R20" s="16">
-        <v>0</v>
-      </c>
-      <c r="S20" s="25"/>
+        <v>0.01</v>
+      </c>
       <c r="T20" s="25"/>
       <c r="U20" s="25"/>
       <c r="V20" s="25"/>
@@ -4113,109 +4133,109 @@
       <c r="Z20" s="25"/>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>43501</v>
-      </c>
-      <c r="B21" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="C21" s="16">
-        <v>3</v>
-      </c>
-      <c r="D21" s="22">
-        <v>3488.8500000265899</v>
-      </c>
-      <c r="E21" s="23">
-        <v>7.9930495221546494E-2</v>
-      </c>
-      <c r="F21" s="37">
-        <v>44367.659999984397</v>
-      </c>
-      <c r="G21" s="16">
+      <c r="A21" s="40">
+        <v>43521</v>
+      </c>
+      <c r="B21" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="41">
+        <v>6</v>
+      </c>
+      <c r="D21" s="41">
+        <v>965.35000000174398</v>
+      </c>
+      <c r="E21" s="42">
+        <v>0.19219790675547099</v>
+      </c>
+      <c r="F21" s="41">
+        <v>5638.6199999970104</v>
+      </c>
+      <c r="G21" s="41">
+        <v>74</v>
+      </c>
+      <c r="H21" s="41">
+        <v>53</v>
+      </c>
+      <c r="I21" s="41">
+        <v>0</v>
+      </c>
+      <c r="J21" s="41">
         <v>59</v>
       </c>
-      <c r="H21" s="16">
-        <v>40</v>
-      </c>
-      <c r="I21" s="16">
-        <v>0</v>
-      </c>
-      <c r="J21" s="16">
-        <v>57</v>
-      </c>
-      <c r="K21" s="16">
-        <v>41</v>
-      </c>
-      <c r="L21" s="16">
-        <v>0</v>
-      </c>
-      <c r="M21" s="16">
-        <v>61</v>
-      </c>
-      <c r="N21" s="16">
-        <v>39</v>
-      </c>
-      <c r="O21" s="16">
-        <v>0</v>
-      </c>
-      <c r="P21" s="16">
-        <v>57</v>
-      </c>
-      <c r="Q21" s="16">
-        <v>47</v>
-      </c>
-      <c r="R21" s="16">
+      <c r="K21" s="41">
+        <v>43</v>
+      </c>
+      <c r="L21" s="41">
+        <v>0</v>
+      </c>
+      <c r="M21" s="41">
+        <v>72</v>
+      </c>
+      <c r="N21" s="41">
+        <v>48</v>
+      </c>
+      <c r="O21" s="41">
+        <v>0</v>
+      </c>
+      <c r="P21" s="41">
+        <v>59</v>
+      </c>
+      <c r="Q21" s="41">
+        <v>47</v>
+      </c>
+      <c r="R21" s="41">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>43502</v>
+        <v>43522</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C22" s="16">
-        <v>3</v>
-      </c>
-      <c r="D22" s="22">
-        <v>3301.1300000168299</v>
-      </c>
-      <c r="E22" s="23">
-        <v>7.5958793595631097E-2</v>
-      </c>
-      <c r="F22" s="37">
-        <v>44367.659999984397</v>
+        <v>6</v>
+      </c>
+      <c r="D22" s="28">
+        <v>507.69999999508298</v>
+      </c>
+      <c r="E22" s="29">
+        <v>0.10371075166508099</v>
+      </c>
+      <c r="F22" s="38">
+        <v>5638.6199999970104</v>
       </c>
       <c r="G22" s="16">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="H22" s="16">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="I22" s="16">
         <v>0</v>
       </c>
       <c r="J22" s="16">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="K22" s="16">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="L22" s="16">
         <v>0</v>
       </c>
       <c r="M22" s="16">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="N22" s="16">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="O22" s="16">
         <v>0</v>
       </c>
       <c r="P22" s="16">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="Q22" s="16">
         <v>47</v>
@@ -4223,7 +4243,6 @@
       <c r="R22" s="16">
         <v>0</v>
       </c>
-      <c r="S22" s="26"/>
       <c r="T22" s="26"/>
       <c r="U22" s="26"/>
       <c r="V22" s="26"/>
@@ -4234,52 +4253,52 @@
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>43503</v>
+        <v>43523</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C23" s="16">
-        <v>4</v>
-      </c>
-      <c r="D23" s="24">
-        <v>1155.59999999918</v>
-      </c>
-      <c r="E23" s="25">
-        <v>9.00398406374502E-2</v>
+        <v>6</v>
+      </c>
+      <c r="D23" s="28">
+        <v>484.89999999657101</v>
+      </c>
+      <c r="E23" s="29">
+        <v>9.3244529019980996E-2</v>
       </c>
       <c r="F23" s="38">
-        <v>13881.470000005</v>
+        <v>5638.6199999970104</v>
       </c>
       <c r="G23" s="16">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="H23" s="16">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="I23" s="16">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="J23" s="16">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="K23" s="16">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="L23" s="16">
         <v>0</v>
       </c>
       <c r="M23" s="16">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="N23" s="16">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="O23" s="16">
         <v>0</v>
       </c>
       <c r="P23" s="16">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="Q23" s="16">
         <v>47</v>
@@ -4289,61 +4308,6 @@
       </c>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>43504</v>
-      </c>
-      <c r="B24" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" s="16">
-        <v>4</v>
-      </c>
-      <c r="D24" s="24">
-        <v>2579.72000000463</v>
-      </c>
-      <c r="E24" s="41">
-        <v>0.19003984063745</v>
-      </c>
-      <c r="F24" s="38">
-        <v>13881.470000005</v>
-      </c>
-      <c r="G24" s="16">
-        <v>58</v>
-      </c>
-      <c r="H24" s="16">
-        <v>44</v>
-      </c>
-      <c r="I24" s="16">
-        <v>0.09</v>
-      </c>
-      <c r="J24" s="16">
-        <v>58</v>
-      </c>
-      <c r="K24" s="16">
-        <v>41</v>
-      </c>
-      <c r="L24" s="16">
-        <v>0.01</v>
-      </c>
-      <c r="M24" s="16">
-        <v>59</v>
-      </c>
-      <c r="N24" s="16">
-        <v>46</v>
-      </c>
-      <c r="O24" s="16">
-        <v>0</v>
-      </c>
-      <c r="P24" s="16">
-        <v>57</v>
-      </c>
-      <c r="Q24" s="16">
-        <v>47</v>
-      </c>
-      <c r="R24" s="16">
-        <v>0</v>
-      </c>
-      <c r="S24" s="27"/>
       <c r="T24" s="27"/>
       <c r="U24" s="27"/>
       <c r="V24" s="27"/>
@@ -4352,118 +4316,7 @@
       <c r="Y24" s="27"/>
       <c r="Z24" s="27"/>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
-        <v>43505</v>
-      </c>
-      <c r="B25" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C25" s="16">
-        <v>4</v>
-      </c>
-      <c r="D25" s="24">
-        <v>4517.1100000133702</v>
-      </c>
-      <c r="E25" s="41">
-        <v>0.31434262948207198</v>
-      </c>
-      <c r="F25" s="38">
-        <v>13881.470000005</v>
-      </c>
-      <c r="G25" s="16">
-        <v>58</v>
-      </c>
-      <c r="H25" s="16">
-        <v>52</v>
-      </c>
-      <c r="I25" s="16">
-        <v>0.16</v>
-      </c>
-      <c r="J25" s="16">
-        <v>58</v>
-      </c>
-      <c r="K25" s="16">
-        <v>41</v>
-      </c>
-      <c r="L25" s="16">
-        <v>0</v>
-      </c>
-      <c r="M25" s="16">
-        <v>59</v>
-      </c>
-      <c r="N25" s="16">
-        <v>52</v>
-      </c>
-      <c r="O25" s="16">
-        <v>0</v>
-      </c>
-      <c r="P25" s="16">
-        <v>58</v>
-      </c>
-      <c r="Q25" s="16">
-        <v>47</v>
-      </c>
-      <c r="R25" s="16">
-        <v>0</v>
-      </c>
-    </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
-        <v>43506</v>
-      </c>
-      <c r="B26" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="C26" s="16">
-        <v>4</v>
-      </c>
-      <c r="D26" s="24">
-        <v>2498.5600000025001</v>
-      </c>
-      <c r="E26" s="41">
-        <v>0.17211155378486101</v>
-      </c>
-      <c r="F26" s="38">
-        <v>13881.470000005</v>
-      </c>
-      <c r="G26" s="16">
-        <v>58</v>
-      </c>
-      <c r="H26" s="16">
-        <v>46</v>
-      </c>
-      <c r="I26" s="16">
-        <v>1.32</v>
-      </c>
-      <c r="J26" s="16">
-        <v>58</v>
-      </c>
-      <c r="K26" s="16">
-        <v>41</v>
-      </c>
-      <c r="L26" s="16">
-        <v>0</v>
-      </c>
-      <c r="M26" s="16">
-        <v>61</v>
-      </c>
-      <c r="N26" s="16">
-        <v>50</v>
-      </c>
-      <c r="O26" s="16">
-        <v>0</v>
-      </c>
-      <c r="P26" s="16">
-        <v>58</v>
-      </c>
-      <c r="Q26" s="16">
-        <v>47</v>
-      </c>
-      <c r="R26" s="16">
-        <v>0</v>
-      </c>
-      <c r="S26" s="28"/>
       <c r="T26" s="28"/>
       <c r="U26" s="28"/>
       <c r="V26" s="28"/>
@@ -4472,174 +4325,7 @@
       <c r="Y26" s="28"/>
       <c r="Z26" s="28"/>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
-        <v>43507</v>
-      </c>
-      <c r="B27" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="C27" s="16">
-        <v>4</v>
-      </c>
-      <c r="D27" s="24">
-        <v>1142.9499999990801</v>
-      </c>
-      <c r="E27" s="25">
-        <v>8.4063745019920297E-2</v>
-      </c>
-      <c r="F27" s="38">
-        <v>13881.470000005</v>
-      </c>
-      <c r="G27" s="16">
-        <v>59</v>
-      </c>
-      <c r="H27" s="16">
-        <v>39</v>
-      </c>
-      <c r="I27" s="16">
-        <v>0</v>
-      </c>
-      <c r="J27" s="16">
-        <v>58</v>
-      </c>
-      <c r="K27" s="16">
-        <v>41</v>
-      </c>
-      <c r="L27" s="16">
-        <v>0</v>
-      </c>
-      <c r="M27" s="16">
-        <v>61</v>
-      </c>
-      <c r="N27" s="16">
-        <v>46</v>
-      </c>
-      <c r="O27" s="16">
-        <v>0</v>
-      </c>
-      <c r="P27" s="16">
-        <v>58</v>
-      </c>
-      <c r="Q27" s="16">
-        <v>47</v>
-      </c>
-      <c r="R27" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
-        <v>43508</v>
-      </c>
-      <c r="B28" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="C28" s="16">
-        <v>4</v>
-      </c>
-      <c r="D28" s="24">
-        <v>1002.49999999639</v>
-      </c>
-      <c r="E28" s="25">
-        <v>7.2908366533864497E-2</v>
-      </c>
-      <c r="F28" s="38">
-        <v>13881.470000005</v>
-      </c>
-      <c r="G28" s="16">
-        <v>65</v>
-      </c>
-      <c r="H28" s="16">
-        <v>44</v>
-      </c>
-      <c r="I28" s="16">
-        <v>0</v>
-      </c>
-      <c r="J28" s="16">
-        <v>58</v>
-      </c>
-      <c r="K28" s="16">
-        <v>41</v>
-      </c>
-      <c r="L28" s="16">
-        <v>0.01</v>
-      </c>
-      <c r="M28" s="16">
-        <v>64</v>
-      </c>
-      <c r="N28" s="16">
-        <v>45</v>
-      </c>
-      <c r="O28" s="16">
-        <v>0</v>
-      </c>
-      <c r="P28" s="16">
-        <v>58</v>
-      </c>
-      <c r="Q28" s="16">
-        <v>47</v>
-      </c>
-      <c r="R28" s="16">
-        <v>0</v>
-      </c>
-    </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
-        <v>43509</v>
-      </c>
-      <c r="B29" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="C29" s="16">
-        <v>4</v>
-      </c>
-      <c r="D29" s="24">
-        <v>985.02999998989696</v>
-      </c>
-      <c r="E29" s="25">
-        <v>7.6494023904382494E-2</v>
-      </c>
-      <c r="F29" s="38">
-        <v>13881.470000005</v>
-      </c>
-      <c r="G29" s="16">
-        <v>67</v>
-      </c>
-      <c r="H29" s="16">
-        <v>46</v>
-      </c>
-      <c r="I29" s="16">
-        <v>0</v>
-      </c>
-      <c r="J29" s="16">
-        <v>58</v>
-      </c>
-      <c r="K29" s="16">
-        <v>41</v>
-      </c>
-      <c r="L29" s="16">
-        <v>0</v>
-      </c>
-      <c r="M29" s="16">
-        <v>64</v>
-      </c>
-      <c r="N29" s="16">
-        <v>46</v>
-      </c>
-      <c r="O29" s="16">
-        <v>0</v>
-      </c>
-      <c r="P29" s="16">
-        <v>58</v>
-      </c>
-      <c r="Q29" s="16">
-        <v>47</v>
-      </c>
-      <c r="R29" s="16">
-        <v>0</v>
-      </c>
-      <c r="S29" s="29"/>
       <c r="T29" s="29"/>
       <c r="U29" s="29"/>
       <c r="V29" s="29"/>
@@ -4648,790 +4334,6 @@
       <c r="Y29" s="29"/>
       <c r="Z29" s="29"/>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A30" s="42">
-        <v>43510</v>
-      </c>
-      <c r="B30" s="43" t="s">
-        <v>4</v>
-      </c>
-      <c r="C30" s="43">
-        <v>5</v>
-      </c>
-      <c r="D30" s="43">
-        <v>925.920000002954</v>
-      </c>
-      <c r="E30" s="44">
-        <v>0.116642958748222</v>
-      </c>
-      <c r="F30" s="43">
-        <v>7839.4899999872496</v>
-      </c>
-      <c r="G30" s="43">
-        <v>70</v>
-      </c>
-      <c r="H30" s="43">
-        <v>50</v>
-      </c>
-      <c r="I30" s="43">
-        <v>0</v>
-      </c>
-      <c r="J30" s="43">
-        <v>58</v>
-      </c>
-      <c r="K30" s="43">
-        <v>41</v>
-      </c>
-      <c r="L30" s="43">
-        <v>0</v>
-      </c>
-      <c r="M30" s="43">
-        <v>66</v>
-      </c>
-      <c r="N30" s="43">
-        <v>46</v>
-      </c>
-      <c r="O30" s="43">
-        <v>0</v>
-      </c>
-      <c r="P30" s="43">
-        <v>58</v>
-      </c>
-      <c r="Q30" s="43">
-        <v>47</v>
-      </c>
-      <c r="R30" s="43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
-        <v>43511</v>
-      </c>
-      <c r="B31" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C31" s="16">
-        <v>5</v>
-      </c>
-      <c r="D31" s="26">
-        <v>1003.94999999598</v>
-      </c>
-      <c r="E31" s="27">
-        <v>0.126600284495021</v>
-      </c>
-      <c r="F31" s="39">
-        <v>7839.4899999872496</v>
-      </c>
-      <c r="G31" s="16">
-        <v>66</v>
-      </c>
-      <c r="H31" s="16">
-        <v>49</v>
-      </c>
-      <c r="I31" s="16">
-        <v>0</v>
-      </c>
-      <c r="J31" s="16">
-        <v>58</v>
-      </c>
-      <c r="K31" s="16">
-        <v>41</v>
-      </c>
-      <c r="L31" s="16">
-        <v>0</v>
-      </c>
-      <c r="M31" s="16">
-        <v>63</v>
-      </c>
-      <c r="N31" s="16">
-        <v>48</v>
-      </c>
-      <c r="O31" s="16">
-        <v>0</v>
-      </c>
-      <c r="P31" s="16">
-        <v>58</v>
-      </c>
-      <c r="Q31" s="16">
-        <v>47</v>
-      </c>
-      <c r="R31" s="16">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
-        <v>43512</v>
-      </c>
-      <c r="B32" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C32" s="16">
-        <v>5</v>
-      </c>
-      <c r="D32" s="26">
-        <v>2388.7100000123201</v>
-      </c>
-      <c r="E32" s="41">
-        <v>0.29302987197724001</v>
-      </c>
-      <c r="F32" s="39">
-        <v>7839.4899999872496</v>
-      </c>
-      <c r="G32" s="16">
-        <v>68</v>
-      </c>
-      <c r="H32" s="16">
-        <v>45</v>
-      </c>
-      <c r="I32" s="16">
-        <v>0</v>
-      </c>
-      <c r="J32" s="16">
-        <v>58</v>
-      </c>
-      <c r="K32" s="16">
-        <v>41</v>
-      </c>
-      <c r="L32" s="16">
-        <v>0.01</v>
-      </c>
-      <c r="M32" s="16">
-        <v>66</v>
-      </c>
-      <c r="N32" s="16">
-        <v>50</v>
-      </c>
-      <c r="O32" s="16">
-        <v>0</v>
-      </c>
-      <c r="P32" s="16">
-        <v>58</v>
-      </c>
-      <c r="Q32" s="16">
-        <v>47</v>
-      </c>
-      <c r="R32" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
-        <v>43513</v>
-      </c>
-      <c r="B33" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="C33" s="16">
-        <v>5</v>
-      </c>
-      <c r="D33" s="26">
-        <v>1468.7300000012201</v>
-      </c>
-      <c r="E33" s="41">
-        <v>0.17567567567567599</v>
-      </c>
-      <c r="F33" s="39">
-        <v>7839.4899999872496</v>
-      </c>
-      <c r="G33" s="16">
-        <v>62</v>
-      </c>
-      <c r="H33" s="16">
-        <v>47</v>
-      </c>
-      <c r="I33" s="16">
-        <v>0.13</v>
-      </c>
-      <c r="J33" s="16">
-        <v>58</v>
-      </c>
-      <c r="K33" s="16">
-        <v>41</v>
-      </c>
-      <c r="L33" s="16">
-        <v>0</v>
-      </c>
-      <c r="M33" s="16">
-        <v>61</v>
-      </c>
-      <c r="N33" s="16">
-        <v>46</v>
-      </c>
-      <c r="O33" s="16">
-        <v>0</v>
-      </c>
-      <c r="P33" s="16">
-        <v>58</v>
-      </c>
-      <c r="Q33" s="16">
-        <v>47</v>
-      </c>
-      <c r="R33" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A34" s="42">
-        <v>43514</v>
-      </c>
-      <c r="B34" s="43" t="s">
-        <v>8</v>
-      </c>
-      <c r="C34" s="43">
-        <v>5</v>
-      </c>
-      <c r="D34" s="43">
-        <v>960.89999999244696</v>
-      </c>
-      <c r="E34" s="44">
-        <v>0.139402560455192</v>
-      </c>
-      <c r="F34" s="43">
-        <v>7839.4899999872496</v>
-      </c>
-      <c r="G34" s="43">
-        <v>59</v>
-      </c>
-      <c r="H34" s="43">
-        <v>45</v>
-      </c>
-      <c r="I34" s="43">
-        <v>0.3</v>
-      </c>
-      <c r="J34" s="43">
-        <v>58</v>
-      </c>
-      <c r="K34" s="43">
-        <v>42</v>
-      </c>
-      <c r="L34" s="43">
-        <v>0</v>
-      </c>
-      <c r="M34" s="43">
-        <v>54</v>
-      </c>
-      <c r="N34" s="43">
-        <v>48</v>
-      </c>
-      <c r="O34" s="43">
-        <v>0</v>
-      </c>
-      <c r="P34" s="43">
-        <v>58</v>
-      </c>
-      <c r="Q34" s="43">
-        <v>47</v>
-      </c>
-      <c r="R34" s="43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
-        <v>43515</v>
-      </c>
-      <c r="B35" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="C35" s="16">
-        <v>5</v>
-      </c>
-      <c r="D35" s="26">
-        <v>458.800000008724</v>
-      </c>
-      <c r="E35" s="27">
-        <v>6.1166429587482203E-2</v>
-      </c>
-      <c r="F35" s="39">
-        <v>7839.4899999872496</v>
-      </c>
-      <c r="G35" s="16">
-        <v>56</v>
-      </c>
-      <c r="H35" s="16">
-        <v>38</v>
-      </c>
-      <c r="I35" s="16">
-        <v>0</v>
-      </c>
-      <c r="J35" s="16">
-        <v>58</v>
-      </c>
-      <c r="K35" s="16">
-        <v>42</v>
-      </c>
-      <c r="L35" s="16">
-        <v>0</v>
-      </c>
-      <c r="M35" s="16">
-        <v>61</v>
-      </c>
-      <c r="N35" s="16">
-        <v>48</v>
-      </c>
-      <c r="O35" s="16">
-        <v>0</v>
-      </c>
-      <c r="P35" s="16">
-        <v>58</v>
-      </c>
-      <c r="Q35" s="16">
-        <v>47</v>
-      </c>
-      <c r="R35" s="16">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
-        <v>43516</v>
-      </c>
-      <c r="B36" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="C36" s="16">
-        <v>5</v>
-      </c>
-      <c r="D36" s="26">
-        <v>632.48000000912396</v>
-      </c>
-      <c r="E36" s="27">
-        <v>8.7482219061166405E-2</v>
-      </c>
-      <c r="F36" s="39">
-        <v>7839.4899999872496</v>
-      </c>
-      <c r="G36" s="16">
-        <v>59</v>
-      </c>
-      <c r="H36" s="16">
-        <v>40</v>
-      </c>
-      <c r="I36" s="16">
-        <v>0</v>
-      </c>
-      <c r="J36" s="16">
-        <v>59</v>
-      </c>
-      <c r="K36" s="16">
-        <v>42</v>
-      </c>
-      <c r="L36" s="16">
-        <v>0.01</v>
-      </c>
-      <c r="M36" s="16">
-        <v>63</v>
-      </c>
-      <c r="N36" s="16">
-        <v>43</v>
-      </c>
-      <c r="O36" s="16">
-        <v>0</v>
-      </c>
-      <c r="P36" s="16">
-        <v>58</v>
-      </c>
-      <c r="Q36" s="16">
-        <v>47</v>
-      </c>
-      <c r="R36" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A37" s="1">
-        <v>43517</v>
-      </c>
-      <c r="B37" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="C37" s="16">
-        <v>6</v>
-      </c>
-      <c r="D37" s="28">
-        <v>445.849999992432</v>
-      </c>
-      <c r="E37" s="29">
-        <v>7.9923882017126593E-2</v>
-      </c>
-      <c r="F37" s="40">
-        <v>5638.6199999970104</v>
-      </c>
-      <c r="G37" s="16">
-        <v>66</v>
-      </c>
-      <c r="H37" s="16">
-        <v>47</v>
-      </c>
-      <c r="I37" s="16">
-        <v>0</v>
-      </c>
-      <c r="J37" s="16">
-        <v>59</v>
-      </c>
-      <c r="K37" s="16">
-        <v>42</v>
-      </c>
-      <c r="L37" s="16">
-        <v>0</v>
-      </c>
-      <c r="M37" s="16">
-        <v>64</v>
-      </c>
-      <c r="N37" s="16">
-        <v>45</v>
-      </c>
-      <c r="O37" s="16">
-        <v>0</v>
-      </c>
-      <c r="P37" s="16">
-        <v>58</v>
-      </c>
-      <c r="Q37" s="16">
-        <v>47</v>
-      </c>
-      <c r="R37" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A38" s="1">
-        <v>43518</v>
-      </c>
-      <c r="B38" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C38" s="16">
-        <v>6</v>
-      </c>
-      <c r="D38" s="28">
-        <v>881.74000000072999</v>
-      </c>
-      <c r="E38" s="41">
-        <v>0.14367269267364399</v>
-      </c>
-      <c r="F38" s="40">
-        <v>5638.6199999970104</v>
-      </c>
-      <c r="G38" s="16">
-        <v>73</v>
-      </c>
-      <c r="H38" s="16">
-        <v>49</v>
-      </c>
-      <c r="I38" s="16">
-        <v>0</v>
-      </c>
-      <c r="J38" s="16">
-        <v>59</v>
-      </c>
-      <c r="K38" s="16">
-        <v>42</v>
-      </c>
-      <c r="L38" s="16">
-        <v>0</v>
-      </c>
-      <c r="M38" s="16">
-        <v>68</v>
-      </c>
-      <c r="N38" s="16">
-        <v>50</v>
-      </c>
-      <c r="O38" s="16">
-        <v>0</v>
-      </c>
-      <c r="P38" s="16">
-        <v>59</v>
-      </c>
-      <c r="Q38" s="16">
-        <v>47</v>
-      </c>
-      <c r="R38" s="16">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A39" s="1">
-        <v>43519</v>
-      </c>
-      <c r="B39" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C39" s="16">
-        <v>6</v>
-      </c>
-      <c r="D39" s="28">
-        <v>1348.8000000028901</v>
-      </c>
-      <c r="E39" s="41">
-        <v>0.22359657469077099</v>
-      </c>
-      <c r="F39" s="40">
-        <v>5638.6199999970104</v>
-      </c>
-      <c r="G39" s="16">
-        <v>72</v>
-      </c>
-      <c r="H39" s="16">
-        <v>50</v>
-      </c>
-      <c r="I39" s="16">
-        <v>0</v>
-      </c>
-      <c r="J39" s="16">
-        <v>59</v>
-      </c>
-      <c r="K39" s="16">
-        <v>42</v>
-      </c>
-      <c r="L39" s="16">
-        <v>0</v>
-      </c>
-      <c r="M39" s="16">
-        <v>70</v>
-      </c>
-      <c r="N39" s="16">
-        <v>48</v>
-      </c>
-      <c r="O39" s="16">
-        <v>0</v>
-      </c>
-      <c r="P39" s="16">
-        <v>59</v>
-      </c>
-      <c r="Q39" s="16">
-        <v>47</v>
-      </c>
-      <c r="R39" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A40" s="1">
-        <v>43520</v>
-      </c>
-      <c r="B40" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="C40" s="16">
-        <v>6</v>
-      </c>
-      <c r="D40" s="28">
-        <v>1004.27999998993</v>
-      </c>
-      <c r="E40" s="41">
-        <v>0.16365366317792601</v>
-      </c>
-      <c r="F40" s="40">
-        <v>5638.6199999970104</v>
-      </c>
-      <c r="G40" s="16">
-        <v>74</v>
-      </c>
-      <c r="H40" s="16">
-        <v>51</v>
-      </c>
-      <c r="I40" s="16">
-        <v>0</v>
-      </c>
-      <c r="J40" s="16">
-        <v>59</v>
-      </c>
-      <c r="K40" s="16">
-        <v>43</v>
-      </c>
-      <c r="L40" s="16">
-        <v>0.01</v>
-      </c>
-      <c r="M40" s="16">
-        <v>70</v>
-      </c>
-      <c r="N40" s="16">
-        <v>46</v>
-      </c>
-      <c r="O40" s="16">
-        <v>0</v>
-      </c>
-      <c r="P40" s="16">
-        <v>59</v>
-      </c>
-      <c r="Q40" s="16">
-        <v>47</v>
-      </c>
-      <c r="R40" s="16">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A41" s="42">
-        <v>43521</v>
-      </c>
-      <c r="B41" s="43" t="s">
-        <v>8</v>
-      </c>
-      <c r="C41" s="43">
-        <v>6</v>
-      </c>
-      <c r="D41" s="43">
-        <v>965.35000000174398</v>
-      </c>
-      <c r="E41" s="44">
-        <v>0.19219790675547099</v>
-      </c>
-      <c r="F41" s="43">
-        <v>5638.6199999970104</v>
-      </c>
-      <c r="G41" s="43">
-        <v>74</v>
-      </c>
-      <c r="H41" s="43">
-        <v>53</v>
-      </c>
-      <c r="I41" s="43">
-        <v>0</v>
-      </c>
-      <c r="J41" s="43">
-        <v>59</v>
-      </c>
-      <c r="K41" s="43">
-        <v>43</v>
-      </c>
-      <c r="L41" s="43">
-        <v>0</v>
-      </c>
-      <c r="M41" s="43">
-        <v>72</v>
-      </c>
-      <c r="N41" s="43">
-        <v>48</v>
-      </c>
-      <c r="O41" s="43">
-        <v>0</v>
-      </c>
-      <c r="P41" s="43">
-        <v>59</v>
-      </c>
-      <c r="Q41" s="43">
-        <v>47</v>
-      </c>
-      <c r="R41" s="43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A42" s="1">
-        <v>43522</v>
-      </c>
-      <c r="B42" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="C42" s="16">
-        <v>6</v>
-      </c>
-      <c r="D42" s="28">
-        <v>507.69999999508298</v>
-      </c>
-      <c r="E42" s="29">
-        <v>0.10371075166508099</v>
-      </c>
-      <c r="F42" s="40">
-        <v>5638.6199999970104</v>
-      </c>
-      <c r="G42" s="16">
-        <v>75</v>
-      </c>
-      <c r="H42" s="16">
-        <v>52</v>
-      </c>
-      <c r="I42" s="16">
-        <v>0</v>
-      </c>
-      <c r="J42" s="16">
-        <v>59</v>
-      </c>
-      <c r="K42" s="16">
-        <v>43</v>
-      </c>
-      <c r="L42" s="16">
-        <v>0</v>
-      </c>
-      <c r="M42" s="16">
-        <v>68</v>
-      </c>
-      <c r="N42" s="16">
-        <v>48</v>
-      </c>
-      <c r="O42" s="16">
-        <v>0</v>
-      </c>
-      <c r="P42" s="16">
-        <v>59</v>
-      </c>
-      <c r="Q42" s="16">
-        <v>47</v>
-      </c>
-      <c r="R42" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A43" s="1">
-        <v>43523</v>
-      </c>
-      <c r="B43" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="C43" s="16">
-        <v>6</v>
-      </c>
-      <c r="D43" s="28">
-        <v>484.89999999657101</v>
-      </c>
-      <c r="E43" s="29">
-        <v>9.3244529019980996E-2</v>
-      </c>
-      <c r="F43" s="40">
-        <v>5638.6199999970104</v>
-      </c>
-      <c r="G43" s="16">
-        <v>64</v>
-      </c>
-      <c r="H43" s="16">
-        <v>49</v>
-      </c>
-      <c r="I43" s="16">
-        <v>0.02</v>
-      </c>
-      <c r="J43" s="16">
-        <v>59</v>
-      </c>
-      <c r="K43" s="16">
-        <v>43</v>
-      </c>
-      <c r="L43" s="16">
-        <v>0</v>
-      </c>
-      <c r="M43" s="16">
-        <v>63</v>
-      </c>
-      <c r="N43" s="16">
-        <v>50</v>
-      </c>
-      <c r="O43" s="16">
-        <v>0</v>
-      </c>
-      <c r="P43" s="16">
-        <v>59</v>
-      </c>
-      <c r="Q43" s="16">
-        <v>47</v>
-      </c>
-      <c r="R43" s="16">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>